<commit_message>
Se actualizo el cronograma, se agrego el pocentaje de tiempo invertido a cada actividad
</commit_message>
<xml_diff>
--- a/Documentacion/CronogramaEQ4.xlsx
+++ b/Documentacion/CronogramaEQ4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\6Semester\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro Yo Mero xd\Documents\ProyectoDomotica\proyectoDomotica\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E107B6-044E-482E-B0B8-42D16C36D6A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D310B7FC-E27A-44B0-B577-06DBE98EFDFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t xml:space="preserve">Actividad </t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>Preparación ESP32 y Git</t>
-  </si>
-  <si>
-    <t>Recopilación de información para documentacion</t>
   </si>
   <si>
     <t>Ensamblar y montar la estructura del proyecto</t>
@@ -256,6 +253,15 @@
       <t xml:space="preserve"> Se encuentra para utilizarlo en caso de que suceda algún imprevisto durante la elaboración del proyecto.</t>
     </r>
   </si>
+  <si>
+    <t>Actividad</t>
+  </si>
+  <si>
+    <t>Pocentaje de tiempo invertido</t>
+  </si>
+  <si>
+    <t>Recopilación de información para documentación</t>
+  </si>
 </sst>
 </file>
 
@@ -408,7 +414,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -431,12 +437,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -510,14 +542,41 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -742,57 +801,57 @@
   <dimension ref="A1:M218"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.375" defaultRowHeight="15.05" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.375" customWidth="1"/>
-    <col min="2" max="12" width="10.25" customWidth="1"/>
+    <col min="1" max="1" width="39.33203125" customWidth="1"/>
+    <col min="2" max="12" width="10.21875" customWidth="1"/>
     <col min="13" max="13" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
+    <row r="1" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26" t="s">
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="26"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29"/>
       <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
@@ -827,7 +886,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>16</v>
       </c>
@@ -843,7 +902,7 @@
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
     </row>
-    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>15</v>
       </c>
@@ -859,9 +918,9 @@
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:13" ht="27.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="27.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -875,9 +934,9 @@
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
     </row>
-    <row r="7" spans="1:13" ht="26.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="26.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="7"/>
@@ -891,9 +950,9 @@
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="7"/>
@@ -907,9 +966,9 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="7"/>
@@ -923,9 +982,9 @@
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
     </row>
-    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
@@ -939,9 +998,9 @@
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
     </row>
-    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="7"/>
@@ -955,9 +1014,9 @@
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
     </row>
-    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
@@ -971,9 +1030,9 @@
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
     </row>
-    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -987,9 +1046,9 @@
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
     </row>
-    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1003,7 +1062,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1017,191 +1076,191 @@
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="25" t="s">
+    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+    </row>
+    <row r="17" spans="1:13" ht="32.700000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
-    </row>
-    <row r="17" spans="1:13" ht="32.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="25" t="s">
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+    </row>
+    <row r="18" spans="1:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-    </row>
-    <row r="18" spans="1:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="25" t="s">
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+    </row>
+    <row r="19" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
-    </row>
-    <row r="19" spans="1:13" ht="17.05" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="25" t="s">
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="1:13" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="25" t="s">
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
-      <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="25" t="s">
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="1"/>
-    </row>
-    <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="25" t="s">
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="1"/>
+    </row>
+    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="1"/>
-    </row>
-    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="25" t="s">
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="1"/>
-    </row>
-    <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="25" t="s">
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="1"/>
+    </row>
+    <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="1"/>
-    </row>
-    <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="25" t="s">
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="27"/>
+      <c r="M25" s="1"/>
+    </row>
+    <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="1"/>
-    </row>
-    <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="25"/>
-      <c r="L26" s="25"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="27"/>
       <c r="M26" s="1"/>
     </row>
-    <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
       <c r="B27" s="24"/>
       <c r="C27" s="24"/>
@@ -1216,7 +1275,7 @@
       <c r="L27" s="24"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1230,7 +1289,7 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1244,9 +1303,14 @@
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+    <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="36"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -1258,9 +1322,10 @@
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
+    <row r="31" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="30"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -1272,9 +1337,14 @@
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
+    <row r="32" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="35">
+        <v>0.05</v>
+      </c>
+      <c r="C32" s="32"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -1286,9 +1356,14 @@
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
     </row>
-    <row r="33" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
+    <row r="33" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="34">
+        <v>0.05</v>
+      </c>
+      <c r="C33" s="33"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -1300,9 +1375,14 @@
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
     </row>
-    <row r="34" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
+    <row r="34" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="35">
+        <v>0.05</v>
+      </c>
+      <c r="C34" s="32"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -1314,9 +1394,14 @@
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
     </row>
-    <row r="35" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
+    <row r="35" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="34">
+        <v>0.15</v>
+      </c>
+      <c r="C35" s="33"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -1328,9 +1413,14 @@
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
     </row>
-    <row r="36" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
+    <row r="36" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" s="34">
+        <v>0.1</v>
+      </c>
+      <c r="C36" s="33"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -1342,9 +1432,14 @@
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
+    <row r="37" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="34">
+        <v>0.1</v>
+      </c>
+      <c r="C37" s="33"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -1356,9 +1451,14 @@
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
     </row>
-    <row r="38" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
+    <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="34">
+        <v>0.08</v>
+      </c>
+      <c r="C38" s="33"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -1370,9 +1470,14 @@
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
     </row>
-    <row r="39" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
+    <row r="39" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="34">
+        <v>0.15</v>
+      </c>
+      <c r="C39" s="33"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -1384,9 +1489,14 @@
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
     </row>
-    <row r="40" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
+    <row r="40" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="34">
+        <v>0.1</v>
+      </c>
+      <c r="C40" s="33"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -1398,9 +1508,14 @@
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
     </row>
-    <row r="41" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
+    <row r="41" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="34">
+        <v>0.1</v>
+      </c>
+      <c r="C41" s="33"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -1412,9 +1527,14 @@
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
     </row>
-    <row r="42" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
+    <row r="42" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="34">
+        <v>0.04</v>
+      </c>
+      <c r="C42" s="33"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -1426,7 +1546,7 @@
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
     </row>
-    <row r="43" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -1440,7 +1560,7 @@
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
     </row>
-    <row r="44" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -1454,7 +1574,7 @@
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
     </row>
-    <row r="45" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -1468,7 +1588,7 @@
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
     </row>
-    <row r="46" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -1482,7 +1602,7 @@
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
     </row>
-    <row r="47" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -1496,7 +1616,7 @@
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
     </row>
-    <row r="48" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -1510,7 +1630,7 @@
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
     </row>
-    <row r="49" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -1524,7 +1644,7 @@
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
     </row>
-    <row r="50" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -1538,7 +1658,7 @@
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
     </row>
-    <row r="51" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -1552,7 +1672,7 @@
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
     </row>
-    <row r="52" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -1566,7 +1686,7 @@
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
     </row>
-    <row r="53" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -1580,7 +1700,7 @@
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
     </row>
-    <row r="54" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -1594,7 +1714,7 @@
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
     </row>
-    <row r="55" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -1608,7 +1728,7 @@
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
     </row>
-    <row r="56" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -1622,7 +1742,7 @@
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
     </row>
-    <row r="57" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -1636,7 +1756,7 @@
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
     </row>
-    <row r="58" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -1650,7 +1770,7 @@
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
     </row>
-    <row r="59" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -1664,7 +1784,7 @@
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
     </row>
-    <row r="60" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -1678,7 +1798,7 @@
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
     </row>
-    <row r="61" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -1692,7 +1812,7 @@
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
     </row>
-    <row r="62" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -1706,7 +1826,7 @@
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
     </row>
-    <row r="63" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -1720,7 +1840,7 @@
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
     </row>
-    <row r="64" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -1734,7 +1854,7 @@
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
     </row>
-    <row r="65" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -1748,7 +1868,7 @@
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
     </row>
-    <row r="66" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -1762,7 +1882,7 @@
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
     </row>
-    <row r="67" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -1776,7 +1896,7 @@
       <c r="L67" s="1"/>
       <c r="M67" s="1"/>
     </row>
-    <row r="68" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -1790,7 +1910,7 @@
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
     </row>
-    <row r="69" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -1804,7 +1924,7 @@
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
     </row>
-    <row r="70" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -1818,7 +1938,7 @@
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
     </row>
-    <row r="71" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -1832,7 +1952,7 @@
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
     </row>
-    <row r="72" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -1846,7 +1966,7 @@
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
     </row>
-    <row r="73" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
@@ -1860,7 +1980,7 @@
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
     </row>
-    <row r="74" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -1874,7 +1994,7 @@
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
     </row>
-    <row r="75" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -1888,7 +2008,7 @@
       <c r="L75" s="1"/>
       <c r="M75" s="1"/>
     </row>
-    <row r="76" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -1902,7 +2022,7 @@
       <c r="L76" s="1"/>
       <c r="M76" s="1"/>
     </row>
-    <row r="77" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -1916,7 +2036,7 @@
       <c r="L77" s="1"/>
       <c r="M77" s="1"/>
     </row>
-    <row r="78" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -1930,7 +2050,7 @@
       <c r="L78" s="1"/>
       <c r="M78" s="1"/>
     </row>
-    <row r="79" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
@@ -1944,7 +2064,7 @@
       <c r="L79" s="1"/>
       <c r="M79" s="1"/>
     </row>
-    <row r="80" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
@@ -1958,7 +2078,7 @@
       <c r="L80" s="1"/>
       <c r="M80" s="1"/>
     </row>
-    <row r="81" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
@@ -1972,7 +2092,7 @@
       <c r="L81" s="1"/>
       <c r="M81" s="1"/>
     </row>
-    <row r="82" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
@@ -1986,7 +2106,7 @@
       <c r="L82" s="1"/>
       <c r="M82" s="1"/>
     </row>
-    <row r="83" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
@@ -2000,7 +2120,7 @@
       <c r="L83" s="1"/>
       <c r="M83" s="1"/>
     </row>
-    <row r="84" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
@@ -2014,7 +2134,7 @@
       <c r="L84" s="1"/>
       <c r="M84" s="1"/>
     </row>
-    <row r="85" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
@@ -2028,7 +2148,7 @@
       <c r="L85" s="1"/>
       <c r="M85" s="1"/>
     </row>
-    <row r="86" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
@@ -2042,7 +2162,7 @@
       <c r="L86" s="1"/>
       <c r="M86" s="1"/>
     </row>
-    <row r="87" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
@@ -2056,7 +2176,7 @@
       <c r="L87" s="1"/>
       <c r="M87" s="1"/>
     </row>
-    <row r="88" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
@@ -2070,7 +2190,7 @@
       <c r="L88" s="1"/>
       <c r="M88" s="1"/>
     </row>
-    <row r="89" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
@@ -2084,7 +2204,7 @@
       <c r="L89" s="1"/>
       <c r="M89" s="1"/>
     </row>
-    <row r="90" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
@@ -2098,7 +2218,7 @@
       <c r="L90" s="1"/>
       <c r="M90" s="1"/>
     </row>
-    <row r="91" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
@@ -2112,7 +2232,7 @@
       <c r="L91" s="1"/>
       <c r="M91" s="1"/>
     </row>
-    <row r="92" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
@@ -2126,7 +2246,7 @@
       <c r="L92" s="1"/>
       <c r="M92" s="1"/>
     </row>
-    <row r="93" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
@@ -2140,7 +2260,7 @@
       <c r="L93" s="1"/>
       <c r="M93" s="1"/>
     </row>
-    <row r="94" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
@@ -2154,7 +2274,7 @@
       <c r="L94" s="1"/>
       <c r="M94" s="1"/>
     </row>
-    <row r="95" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
@@ -2168,7 +2288,7 @@
       <c r="L95" s="1"/>
       <c r="M95" s="1"/>
     </row>
-    <row r="96" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
@@ -2182,7 +2302,7 @@
       <c r="L96" s="1"/>
       <c r="M96" s="1"/>
     </row>
-    <row r="97" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
@@ -2196,7 +2316,7 @@
       <c r="L97" s="1"/>
       <c r="M97" s="1"/>
     </row>
-    <row r="98" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
@@ -2210,7 +2330,7 @@
       <c r="L98" s="1"/>
       <c r="M98" s="1"/>
     </row>
-    <row r="99" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
@@ -2224,7 +2344,7 @@
       <c r="L99" s="1"/>
       <c r="M99" s="1"/>
     </row>
-    <row r="100" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
@@ -2238,7 +2358,7 @@
       <c r="L100" s="1"/>
       <c r="M100" s="1"/>
     </row>
-    <row r="101" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
@@ -2252,7 +2372,7 @@
       <c r="L101" s="1"/>
       <c r="M101" s="1"/>
     </row>
-    <row r="102" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
@@ -2266,7 +2386,7 @@
       <c r="L102" s="1"/>
       <c r="M102" s="1"/>
     </row>
-    <row r="103" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
@@ -2280,7 +2400,7 @@
       <c r="L103" s="1"/>
       <c r="M103" s="1"/>
     </row>
-    <row r="104" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
@@ -2294,7 +2414,7 @@
       <c r="L104" s="1"/>
       <c r="M104" s="1"/>
     </row>
-    <row r="105" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
@@ -2308,7 +2428,7 @@
       <c r="L105" s="1"/>
       <c r="M105" s="1"/>
     </row>
-    <row r="106" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
@@ -2322,7 +2442,7 @@
       <c r="L106" s="1"/>
       <c r="M106" s="1"/>
     </row>
-    <row r="107" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
@@ -2336,7 +2456,7 @@
       <c r="L107" s="1"/>
       <c r="M107" s="1"/>
     </row>
-    <row r="108" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
@@ -2350,7 +2470,7 @@
       <c r="L108" s="1"/>
       <c r="M108" s="1"/>
     </row>
-    <row r="109" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
@@ -2364,7 +2484,7 @@
       <c r="L109" s="1"/>
       <c r="M109" s="1"/>
     </row>
-    <row r="110" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
@@ -2378,7 +2498,7 @@
       <c r="L110" s="1"/>
       <c r="M110" s="1"/>
     </row>
-    <row r="111" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
@@ -2392,7 +2512,7 @@
       <c r="L111" s="1"/>
       <c r="M111" s="1"/>
     </row>
-    <row r="112" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
@@ -2406,7 +2526,7 @@
       <c r="L112" s="1"/>
       <c r="M112" s="1"/>
     </row>
-    <row r="113" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
@@ -2420,7 +2540,7 @@
       <c r="L113" s="1"/>
       <c r="M113" s="1"/>
     </row>
-    <row r="114" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
@@ -2434,7 +2554,7 @@
       <c r="L114" s="1"/>
       <c r="M114" s="1"/>
     </row>
-    <row r="115" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
@@ -2448,7 +2568,7 @@
       <c r="L115" s="1"/>
       <c r="M115" s="1"/>
     </row>
-    <row r="116" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
@@ -2462,7 +2582,7 @@
       <c r="L116" s="1"/>
       <c r="M116" s="1"/>
     </row>
-    <row r="117" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
@@ -2476,7 +2596,7 @@
       <c r="L117" s="1"/>
       <c r="M117" s="1"/>
     </row>
-    <row r="118" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
@@ -2490,7 +2610,7 @@
       <c r="L118" s="1"/>
       <c r="M118" s="1"/>
     </row>
-    <row r="119" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
@@ -2504,7 +2624,7 @@
       <c r="L119" s="1"/>
       <c r="M119" s="1"/>
     </row>
-    <row r="120" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
@@ -2518,7 +2638,7 @@
       <c r="L120" s="1"/>
       <c r="M120" s="1"/>
     </row>
-    <row r="121" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
@@ -2532,7 +2652,7 @@
       <c r="L121" s="1"/>
       <c r="M121" s="1"/>
     </row>
-    <row r="122" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
@@ -2546,7 +2666,7 @@
       <c r="L122" s="1"/>
       <c r="M122" s="1"/>
     </row>
-    <row r="123" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
@@ -2560,7 +2680,7 @@
       <c r="L123" s="1"/>
       <c r="M123" s="1"/>
     </row>
-    <row r="124" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
@@ -2574,7 +2694,7 @@
       <c r="L124" s="1"/>
       <c r="M124" s="1"/>
     </row>
-    <row r="125" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
@@ -2588,7 +2708,7 @@
       <c r="L125" s="1"/>
       <c r="M125" s="1"/>
     </row>
-    <row r="126" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
@@ -2602,7 +2722,7 @@
       <c r="L126" s="1"/>
       <c r="M126" s="1"/>
     </row>
-    <row r="127" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
@@ -2616,7 +2736,7 @@
       <c r="L127" s="1"/>
       <c r="M127" s="1"/>
     </row>
-    <row r="128" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
@@ -2630,7 +2750,7 @@
       <c r="L128" s="1"/>
       <c r="M128" s="1"/>
     </row>
-    <row r="129" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
@@ -2644,7 +2764,7 @@
       <c r="L129" s="1"/>
       <c r="M129" s="1"/>
     </row>
-    <row r="130" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
@@ -2658,7 +2778,7 @@
       <c r="L130" s="1"/>
       <c r="M130" s="1"/>
     </row>
-    <row r="131" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
@@ -2672,7 +2792,7 @@
       <c r="L131" s="1"/>
       <c r="M131" s="1"/>
     </row>
-    <row r="132" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
@@ -2686,7 +2806,7 @@
       <c r="L132" s="1"/>
       <c r="M132" s="1"/>
     </row>
-    <row r="133" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
@@ -2700,7 +2820,7 @@
       <c r="L133" s="1"/>
       <c r="M133" s="1"/>
     </row>
-    <row r="134" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
@@ -2714,7 +2834,7 @@
       <c r="L134" s="1"/>
       <c r="M134" s="1"/>
     </row>
-    <row r="135" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
@@ -2728,7 +2848,7 @@
       <c r="L135" s="1"/>
       <c r="M135" s="1"/>
     </row>
-    <row r="136" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
       <c r="D136" s="1"/>
@@ -2742,7 +2862,7 @@
       <c r="L136" s="1"/>
       <c r="M136" s="1"/>
     </row>
-    <row r="137" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
@@ -2756,7 +2876,7 @@
       <c r="L137" s="1"/>
       <c r="M137" s="1"/>
     </row>
-    <row r="138" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
@@ -2770,7 +2890,7 @@
       <c r="L138" s="1"/>
       <c r="M138" s="1"/>
     </row>
-    <row r="139" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
@@ -2784,7 +2904,7 @@
       <c r="L139" s="1"/>
       <c r="M139" s="1"/>
     </row>
-    <row r="140" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
@@ -2798,7 +2918,7 @@
       <c r="L140" s="1"/>
       <c r="M140" s="1"/>
     </row>
-    <row r="141" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
       <c r="D141" s="1"/>
@@ -2812,7 +2932,7 @@
       <c r="L141" s="1"/>
       <c r="M141" s="1"/>
     </row>
-    <row r="142" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
@@ -2826,7 +2946,7 @@
       <c r="L142" s="1"/>
       <c r="M142" s="1"/>
     </row>
-    <row r="143" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
@@ -2840,7 +2960,7 @@
       <c r="L143" s="1"/>
       <c r="M143" s="1"/>
     </row>
-    <row r="144" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
       <c r="D144" s="1"/>
@@ -2854,7 +2974,7 @@
       <c r="L144" s="1"/>
       <c r="M144" s="1"/>
     </row>
-    <row r="145" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
       <c r="D145" s="1"/>
@@ -2868,7 +2988,7 @@
       <c r="L145" s="1"/>
       <c r="M145" s="1"/>
     </row>
-    <row r="146" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
       <c r="D146" s="1"/>
@@ -2882,7 +3002,7 @@
       <c r="L146" s="1"/>
       <c r="M146" s="1"/>
     </row>
-    <row r="147" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
       <c r="D147" s="1"/>
@@ -2896,7 +3016,7 @@
       <c r="L147" s="1"/>
       <c r="M147" s="1"/>
     </row>
-    <row r="148" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
       <c r="D148" s="1"/>
@@ -2910,7 +3030,7 @@
       <c r="L148" s="1"/>
       <c r="M148" s="1"/>
     </row>
-    <row r="149" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
       <c r="D149" s="1"/>
@@ -2924,7 +3044,7 @@
       <c r="L149" s="1"/>
       <c r="M149" s="1"/>
     </row>
-    <row r="150" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
       <c r="D150" s="1"/>
@@ -2938,7 +3058,7 @@
       <c r="L150" s="1"/>
       <c r="M150" s="1"/>
     </row>
-    <row r="151" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
       <c r="D151" s="1"/>
@@ -2952,7 +3072,7 @@
       <c r="L151" s="1"/>
       <c r="M151" s="1"/>
     </row>
-    <row r="152" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
       <c r="D152" s="1"/>
@@ -2966,7 +3086,7 @@
       <c r="L152" s="1"/>
       <c r="M152" s="1"/>
     </row>
-    <row r="153" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
       <c r="D153" s="1"/>
@@ -2980,7 +3100,7 @@
       <c r="L153" s="1"/>
       <c r="M153" s="1"/>
     </row>
-    <row r="154" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
       <c r="D154" s="1"/>
@@ -2994,7 +3114,7 @@
       <c r="L154" s="1"/>
       <c r="M154" s="1"/>
     </row>
-    <row r="155" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
       <c r="D155" s="1"/>
@@ -3008,7 +3128,7 @@
       <c r="L155" s="1"/>
       <c r="M155" s="1"/>
     </row>
-    <row r="156" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
       <c r="D156" s="1"/>
@@ -3022,7 +3142,7 @@
       <c r="L156" s="1"/>
       <c r="M156" s="1"/>
     </row>
-    <row r="157" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
       <c r="D157" s="1"/>
@@ -3036,7 +3156,7 @@
       <c r="L157" s="1"/>
       <c r="M157" s="1"/>
     </row>
-    <row r="158" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
       <c r="D158" s="1"/>
@@ -3050,7 +3170,7 @@
       <c r="L158" s="1"/>
       <c r="M158" s="1"/>
     </row>
-    <row r="159" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
       <c r="D159" s="1"/>
@@ -3064,7 +3184,7 @@
       <c r="L159" s="1"/>
       <c r="M159" s="1"/>
     </row>
-    <row r="160" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
       <c r="D160" s="1"/>
@@ -3078,7 +3198,7 @@
       <c r="L160" s="1"/>
       <c r="M160" s="1"/>
     </row>
-    <row r="161" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
       <c r="D161" s="1"/>
@@ -3092,7 +3212,7 @@
       <c r="L161" s="1"/>
       <c r="M161" s="1"/>
     </row>
-    <row r="162" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
       <c r="D162" s="1"/>
@@ -3106,7 +3226,7 @@
       <c r="L162" s="1"/>
       <c r="M162" s="1"/>
     </row>
-    <row r="163" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
       <c r="D163" s="1"/>
@@ -3120,7 +3240,7 @@
       <c r="L163" s="1"/>
       <c r="M163" s="1"/>
     </row>
-    <row r="164" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
       <c r="D164" s="1"/>
@@ -3134,7 +3254,7 @@
       <c r="L164" s="1"/>
       <c r="M164" s="1"/>
     </row>
-    <row r="165" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
       <c r="D165" s="1"/>
@@ -3148,7 +3268,7 @@
       <c r="L165" s="1"/>
       <c r="M165" s="1"/>
     </row>
-    <row r="166" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
       <c r="D166" s="1"/>
@@ -3162,7 +3282,7 @@
       <c r="L166" s="1"/>
       <c r="M166" s="1"/>
     </row>
-    <row r="167" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
       <c r="D167" s="1"/>
@@ -3176,7 +3296,7 @@
       <c r="L167" s="1"/>
       <c r="M167" s="1"/>
     </row>
-    <row r="168" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
       <c r="D168" s="1"/>
@@ -3190,7 +3310,7 @@
       <c r="L168" s="1"/>
       <c r="M168" s="1"/>
     </row>
-    <row r="169" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
       <c r="D169" s="1"/>
@@ -3204,7 +3324,7 @@
       <c r="L169" s="1"/>
       <c r="M169" s="1"/>
     </row>
-    <row r="170" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
       <c r="D170" s="1"/>
@@ -3218,7 +3338,7 @@
       <c r="L170" s="1"/>
       <c r="M170" s="1"/>
     </row>
-    <row r="171" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
       <c r="D171" s="1"/>
@@ -3232,7 +3352,7 @@
       <c r="L171" s="1"/>
       <c r="M171" s="1"/>
     </row>
-    <row r="172" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
       <c r="D172" s="1"/>
@@ -3246,7 +3366,7 @@
       <c r="L172" s="1"/>
       <c r="M172" s="1"/>
     </row>
-    <row r="173" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
       <c r="D173" s="1"/>
@@ -3260,7 +3380,7 @@
       <c r="L173" s="1"/>
       <c r="M173" s="1"/>
     </row>
-    <row r="174" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
       <c r="D174" s="1"/>
@@ -3274,7 +3394,7 @@
       <c r="L174" s="1"/>
       <c r="M174" s="1"/>
     </row>
-    <row r="175" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
       <c r="D175" s="1"/>
@@ -3288,7 +3408,7 @@
       <c r="L175" s="1"/>
       <c r="M175" s="1"/>
     </row>
-    <row r="176" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
       <c r="D176" s="1"/>
@@ -3302,7 +3422,7 @@
       <c r="L176" s="1"/>
       <c r="M176" s="1"/>
     </row>
-    <row r="177" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
       <c r="D177" s="1"/>
@@ -3316,7 +3436,7 @@
       <c r="L177" s="1"/>
       <c r="M177" s="1"/>
     </row>
-    <row r="178" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
       <c r="D178" s="1"/>
@@ -3330,7 +3450,7 @@
       <c r="L178" s="1"/>
       <c r="M178" s="1"/>
     </row>
-    <row r="179" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
       <c r="D179" s="1"/>
@@ -3344,7 +3464,7 @@
       <c r="L179" s="1"/>
       <c r="M179" s="1"/>
     </row>
-    <row r="180" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
       <c r="D180" s="1"/>
@@ -3358,7 +3478,7 @@
       <c r="L180" s="1"/>
       <c r="M180" s="1"/>
     </row>
-    <row r="181" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
       <c r="D181" s="1"/>
@@ -3372,7 +3492,7 @@
       <c r="L181" s="1"/>
       <c r="M181" s="1"/>
     </row>
-    <row r="182" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
       <c r="D182" s="1"/>
@@ -3386,7 +3506,7 @@
       <c r="L182" s="1"/>
       <c r="M182" s="1"/>
     </row>
-    <row r="183" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
       <c r="D183" s="1"/>
@@ -3400,7 +3520,7 @@
       <c r="L183" s="1"/>
       <c r="M183" s="1"/>
     </row>
-    <row r="184" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
       <c r="D184" s="1"/>
@@ -3414,7 +3534,7 @@
       <c r="L184" s="1"/>
       <c r="M184" s="1"/>
     </row>
-    <row r="185" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
       <c r="D185" s="1"/>
@@ -3428,7 +3548,7 @@
       <c r="L185" s="1"/>
       <c r="M185" s="1"/>
     </row>
-    <row r="186" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
       <c r="D186" s="1"/>
@@ -3442,7 +3562,7 @@
       <c r="L186" s="1"/>
       <c r="M186" s="1"/>
     </row>
-    <row r="187" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
       <c r="D187" s="1"/>
@@ -3456,7 +3576,7 @@
       <c r="L187" s="1"/>
       <c r="M187" s="1"/>
     </row>
-    <row r="188" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
       <c r="D188" s="1"/>
@@ -3470,7 +3590,7 @@
       <c r="L188" s="1"/>
       <c r="M188" s="1"/>
     </row>
-    <row r="189" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
       <c r="D189" s="1"/>
@@ -3484,7 +3604,7 @@
       <c r="L189" s="1"/>
       <c r="M189" s="1"/>
     </row>
-    <row r="190" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
       <c r="D190" s="1"/>
@@ -3498,7 +3618,7 @@
       <c r="L190" s="1"/>
       <c r="M190" s="1"/>
     </row>
-    <row r="191" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
       <c r="D191" s="1"/>
@@ -3512,7 +3632,7 @@
       <c r="L191" s="1"/>
       <c r="M191" s="1"/>
     </row>
-    <row r="192" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
       <c r="D192" s="1"/>
@@ -3526,7 +3646,7 @@
       <c r="L192" s="1"/>
       <c r="M192" s="1"/>
     </row>
-    <row r="193" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
       <c r="D193" s="1"/>
@@ -3540,7 +3660,7 @@
       <c r="L193" s="1"/>
       <c r="M193" s="1"/>
     </row>
-    <row r="194" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
       <c r="D194" s="1"/>
@@ -3554,7 +3674,7 @@
       <c r="L194" s="1"/>
       <c r="M194" s="1"/>
     </row>
-    <row r="195" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
       <c r="D195" s="1"/>
@@ -3568,7 +3688,7 @@
       <c r="L195" s="1"/>
       <c r="M195" s="1"/>
     </row>
-    <row r="196" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
       <c r="D196" s="1"/>
@@ -3582,7 +3702,7 @@
       <c r="L196" s="1"/>
       <c r="M196" s="1"/>
     </row>
-    <row r="197" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
       <c r="D197" s="1"/>
@@ -3596,7 +3716,7 @@
       <c r="L197" s="1"/>
       <c r="M197" s="1"/>
     </row>
-    <row r="198" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
       <c r="D198" s="1"/>
@@ -3610,7 +3730,7 @@
       <c r="L198" s="1"/>
       <c r="M198" s="1"/>
     </row>
-    <row r="199" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
       <c r="D199" s="1"/>
@@ -3624,7 +3744,7 @@
       <c r="L199" s="1"/>
       <c r="M199" s="1"/>
     </row>
-    <row r="200" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
       <c r="D200" s="1"/>
@@ -3638,7 +3758,7 @@
       <c r="L200" s="1"/>
       <c r="M200" s="1"/>
     </row>
-    <row r="201" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
       <c r="D201" s="1"/>
@@ -3652,7 +3772,7 @@
       <c r="L201" s="1"/>
       <c r="M201" s="1"/>
     </row>
-    <row r="202" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
       <c r="D202" s="1"/>
@@ -3666,7 +3786,7 @@
       <c r="L202" s="1"/>
       <c r="M202" s="1"/>
     </row>
-    <row r="203" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
       <c r="D203" s="1"/>
@@ -3680,7 +3800,7 @@
       <c r="L203" s="1"/>
       <c r="M203" s="1"/>
     </row>
-    <row r="204" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
       <c r="D204" s="1"/>
@@ -3694,7 +3814,7 @@
       <c r="L204" s="1"/>
       <c r="M204" s="1"/>
     </row>
-    <row r="205" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
       <c r="D205" s="1"/>
@@ -3708,7 +3828,7 @@
       <c r="L205" s="1"/>
       <c r="M205" s="1"/>
     </row>
-    <row r="206" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
       <c r="D206" s="1"/>
@@ -3722,7 +3842,7 @@
       <c r="L206" s="1"/>
       <c r="M206" s="1"/>
     </row>
-    <row r="207" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
       <c r="D207" s="1"/>
@@ -3736,7 +3856,7 @@
       <c r="L207" s="1"/>
       <c r="M207" s="1"/>
     </row>
-    <row r="208" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
       <c r="D208" s="1"/>
@@ -3750,7 +3870,7 @@
       <c r="L208" s="1"/>
       <c r="M208" s="1"/>
     </row>
-    <row r="209" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
       <c r="D209" s="1"/>
@@ -3764,7 +3884,7 @@
       <c r="L209" s="1"/>
       <c r="M209" s="1"/>
     </row>
-    <row r="210" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
       <c r="D210" s="1"/>
@@ -3778,7 +3898,7 @@
       <c r="L210" s="1"/>
       <c r="M210" s="1"/>
     </row>
-    <row r="211" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
       <c r="D211" s="1"/>
@@ -3792,7 +3912,7 @@
       <c r="L211" s="1"/>
       <c r="M211" s="1"/>
     </row>
-    <row r="212" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
       <c r="D212" s="1"/>
@@ -3806,7 +3926,7 @@
       <c r="L212" s="1"/>
       <c r="M212" s="1"/>
     </row>
-    <row r="213" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
       <c r="D213" s="1"/>
@@ -3820,7 +3940,7 @@
       <c r="L213" s="1"/>
       <c r="M213" s="1"/>
     </row>
-    <row r="214" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
       <c r="D214" s="1"/>
@@ -3834,7 +3954,7 @@
       <c r="L214" s="1"/>
       <c r="M214" s="1"/>
     </row>
-    <row r="215" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
       <c r="D215" s="1"/>
@@ -3848,7 +3968,7 @@
       <c r="L215" s="1"/>
       <c r="M215" s="1"/>
     </row>
-    <row r="216" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
       <c r="D216" s="1"/>
@@ -3862,7 +3982,7 @@
       <c r="L216" s="1"/>
       <c r="M216" s="1"/>
     </row>
-    <row r="217" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
       <c r="D217" s="1"/>
@@ -3876,7 +3996,7 @@
       <c r="L217" s="1"/>
       <c r="M217" s="1"/>
     </row>
-    <row r="218" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
       <c r="D218" s="1"/>
@@ -3891,23 +4011,36 @@
       <c r="M218" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A16:L16"/>
-    <mergeCell ref="A17:L17"/>
-    <mergeCell ref="A18:L18"/>
-    <mergeCell ref="A19:L19"/>
-    <mergeCell ref="A20:L20"/>
+  <mergeCells count="29">
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B30:C31"/>
     <mergeCell ref="A26:L26"/>
     <mergeCell ref="A21:L21"/>
     <mergeCell ref="A22:L22"/>
     <mergeCell ref="A23:L23"/>
     <mergeCell ref="A24:L24"/>
     <mergeCell ref="A25:L25"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="A18:L18"/>
+    <mergeCell ref="A19:L19"/>
+    <mergeCell ref="A20:L20"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se agrego el diagrama de Gantt
</commit_message>
<xml_diff>
--- a/Documentacion/CronogramaEQ4.xlsx
+++ b/Documentacion/CronogramaEQ4.xlsx
@@ -5,22 +5,30 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro Yo Mero xd\Documents\ProyectoDomotica\proyectoDomotica\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D310B7FC-E27A-44B0-B577-06DBE98EFDFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35457D5C-C357-4151-B47D-35D8F3A0E164}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t xml:space="preserve">Actividad </t>
   </si>
@@ -86,9 +94,6 @@
   </si>
   <si>
     <t xml:space="preserve">Pruebas finales </t>
-  </si>
-  <si>
-    <t>Tiempo de prórroga</t>
   </si>
   <si>
     <t xml:space="preserve">Preparacion/programación de la base de datos </t>
@@ -254,13 +259,13 @@
     </r>
   </si>
   <si>
-    <t>Actividad</t>
-  </si>
-  <si>
     <t>Pocentaje de tiempo invertido</t>
   </si>
   <si>
     <t>Recopilación de información para documentación</t>
+  </si>
+  <si>
+    <t>Adaptación a la cuarentena</t>
   </si>
 </sst>
 </file>
@@ -367,12 +372,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -413,8 +412,14 @@
         <bgColor rgb="FF6D9EEB"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -463,12 +468,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -506,31 +590,25 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -542,40 +620,95 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -585,6 +718,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFE1771F"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -798,60 +936,68 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M218"/>
+  <dimension ref="A1:O220"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.25" defaultRowHeight="15.05" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.33203125" customWidth="1"/>
-    <col min="2" max="12" width="10.21875" customWidth="1"/>
+    <col min="1" max="1" width="39.25" customWidth="1"/>
+    <col min="2" max="12" width="10.25" customWidth="1"/>
     <col min="13" max="13" width="19" customWidth="1"/>
+    <col min="15" max="15" width="41.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="1"/>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+    <row r="1" spans="1:15" ht="25.55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="32"/>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25" t="s">
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25" t="s">
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="57"/>
+      <c r="O2" s="46"/>
+    </row>
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="52"/>
       <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
@@ -885,13 +1031,16 @@
       <c r="L3" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M3" s="56"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="46"/>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="20"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="18"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -901,13 +1050,18 @@
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
-    </row>
-    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M4" s="47">
+        <v>0.05</v>
+      </c>
+      <c r="N4" s="48"/>
+      <c r="O4" s="23"/>
+    </row>
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="18"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="16"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -917,14 +1071,19 @@
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
-    </row>
-    <row r="6" spans="1:13" ht="27.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>39</v>
+      <c r="M5" s="44">
+        <v>0.05</v>
+      </c>
+      <c r="N5" s="45"/>
+      <c r="O5" s="23"/>
+    </row>
+    <row r="6" spans="1:15" ht="27.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
+        <v>37</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
-      <c r="D6" s="16"/>
+      <c r="D6" s="14"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -933,14 +1092,19 @@
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
-    </row>
-    <row r="7" spans="1:13" ht="26.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M6" s="47">
+        <v>0.05</v>
+      </c>
+      <c r="N6" s="48"/>
+      <c r="O6" s="31"/>
+    </row>
+    <row r="7" spans="1:15" ht="26.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="7"/>
-      <c r="D7" s="15"/>
+      <c r="D7" s="13"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -949,40 +1113,51 @@
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-    </row>
-    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M7" s="44">
+        <v>0.15</v>
+      </c>
+      <c r="N7" s="45"/>
+      <c r="O7" s="23"/>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="38"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="36">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N8" s="34"/>
+      <c r="O8" s="23"/>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="35"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="35"/>
+      <c r="O9" s="23"/>
+    </row>
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>18</v>
       </c>
@@ -997,8 +1172,13 @@
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M10" s="44">
+        <v>0.08</v>
+      </c>
+      <c r="N10" s="45"/>
+      <c r="O10" s="23"/>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>19</v>
       </c>
@@ -1013,8 +1193,13 @@
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
-    </row>
-    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M11" s="44">
+        <v>0.15</v>
+      </c>
+      <c r="N11" s="45"/>
+      <c r="O11" s="23"/>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>20</v>
       </c>
@@ -1029,10 +1214,15 @@
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
-    </row>
-    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M12" s="44">
+        <v>0.1</v>
+      </c>
+      <c r="N12" s="45"/>
+      <c r="O12" s="23"/>
+    </row>
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1042,13 +1232,18 @@
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="9"/>
-      <c r="J13" s="6"/>
+      <c r="J13" s="9"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M13" s="44">
+        <v>0.1</v>
+      </c>
+      <c r="N13" s="45"/>
+      <c r="O13" s="23"/>
+    </row>
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1060,257 +1255,265 @@
       <c r="I14" s="6"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-    </row>
-    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
+      <c r="L14" s="28"/>
+      <c r="M14" s="44">
+        <v>0.1</v>
+      </c>
+      <c r="N14" s="45"/>
+      <c r="O14" s="23"/>
+    </row>
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="44">
+        <v>0.1</v>
+      </c>
+      <c r="N15" s="45"/>
+      <c r="O15" s="32"/>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="23"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="33"/>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="49"/>
+      <c r="L18" s="49"/>
+    </row>
+    <row r="19" spans="1:13" ht="32.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
-    </row>
-    <row r="17" spans="1:13" ht="32.700000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="49"/>
+      <c r="K19" s="49"/>
+      <c r="L19" s="49"/>
+    </row>
+    <row r="20" spans="1:13" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27"/>
-    </row>
-    <row r="18" spans="1:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="49"/>
+    </row>
+    <row r="21" spans="1:13" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="27"/>
-      <c r="L18" s="27"/>
-    </row>
-    <row r="19" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="1:13" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="1:13" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+      <c r="B22" s="49"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="1"/>
+    </row>
+    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="27" t="s">
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="1"/>
-    </row>
-    <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="27" t="s">
+      <c r="B24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="1"/>
+    </row>
+    <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="27"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="27"/>
-      <c r="M22" s="1"/>
-    </row>
-    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="27" t="s">
+      <c r="B25" s="49"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="49"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="1"/>
+    </row>
+    <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="27"/>
-      <c r="M23" s="1"/>
-    </row>
-    <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="27" t="s">
+      <c r="B26" s="49"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="49"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="1"/>
+    </row>
+    <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="1"/>
-    </row>
-    <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
+      <c r="B27" s="49"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="49"/>
+      <c r="L27" s="49"/>
+      <c r="M27" s="1"/>
+    </row>
+    <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="27"/>
-      <c r="L25" s="27"/>
-      <c r="M25" s="1"/>
-    </row>
-    <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="27"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="27"/>
-      <c r="M26" s="1"/>
-    </row>
-    <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="24"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="1"/>
-    </row>
-    <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="49"/>
       <c r="M28" s="1"/>
     </row>
-    <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
+    <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="20"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="22"/>
       <c r="M29" s="1"/>
     </row>
-    <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="36"/>
+    <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -1322,10 +1525,9 @@
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
     </row>
-    <row r="31" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
+    <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -1337,14 +1539,7 @@
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
     </row>
-    <row r="32" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="B32" s="35">
-        <v>0.05</v>
-      </c>
-      <c r="C32" s="32"/>
+    <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -1356,14 +1551,7 @@
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
     </row>
-    <row r="33" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B33" s="34">
-        <v>0.05</v>
-      </c>
-      <c r="C33" s="33"/>
+    <row r="33" spans="2:13" ht="15.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -1375,14 +1563,7 @@
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
     </row>
-    <row r="34" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B34" s="35">
-        <v>0.05</v>
-      </c>
-      <c r="C34" s="32"/>
+    <row r="34" spans="2:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -1394,14 +1575,7 @@
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
     </row>
-    <row r="35" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B35" s="34">
-        <v>0.15</v>
-      </c>
-      <c r="C35" s="33"/>
+    <row r="35" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -1413,14 +1587,7 @@
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
     </row>
-    <row r="36" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B36" s="34">
-        <v>0.1</v>
-      </c>
-      <c r="C36" s="33"/>
+    <row r="36" spans="2:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -1432,14 +1599,7 @@
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
     </row>
-    <row r="37" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B37" s="34">
-        <v>0.1</v>
-      </c>
-      <c r="C37" s="33"/>
+    <row r="37" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -1451,14 +1611,7 @@
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
     </row>
-    <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B38" s="34">
-        <v>0.08</v>
-      </c>
-      <c r="C38" s="33"/>
+    <row r="38" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -1470,14 +1623,7 @@
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
     </row>
-    <row r="39" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B39" s="34">
-        <v>0.15</v>
-      </c>
-      <c r="C39" s="33"/>
+    <row r="39" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -1489,14 +1635,7 @@
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
     </row>
-    <row r="40" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B40" s="34">
-        <v>0.1</v>
-      </c>
-      <c r="C40" s="33"/>
+    <row r="40" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -1508,14 +1647,7 @@
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
     </row>
-    <row r="41" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B41" s="34">
-        <v>0.1</v>
-      </c>
-      <c r="C41" s="33"/>
+    <row r="41" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -1527,14 +1659,7 @@
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
     </row>
-    <row r="42" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B42" s="34">
-        <v>0.04</v>
-      </c>
-      <c r="C42" s="33"/>
+    <row r="42" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -1546,9 +1671,7 @@
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
     </row>
-    <row r="43" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
+    <row r="43" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -1560,9 +1683,7 @@
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
     </row>
-    <row r="44" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
+    <row r="44" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -1574,7 +1695,7 @@
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
     </row>
-    <row r="45" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -1588,7 +1709,7 @@
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
     </row>
-    <row r="46" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -1602,7 +1723,7 @@
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
     </row>
-    <row r="47" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -1616,7 +1737,7 @@
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
     </row>
-    <row r="48" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -1630,7 +1751,7 @@
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
     </row>
-    <row r="49" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -1644,7 +1765,7 @@
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
     </row>
-    <row r="50" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -1658,7 +1779,7 @@
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
     </row>
-    <row r="51" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -1672,7 +1793,7 @@
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
     </row>
-    <row r="52" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -1686,7 +1807,7 @@
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
     </row>
-    <row r="53" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -1700,7 +1821,7 @@
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
     </row>
-    <row r="54" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -1714,7 +1835,7 @@
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
     </row>
-    <row r="55" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -1728,7 +1849,7 @@
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
     </row>
-    <row r="56" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -1742,7 +1863,7 @@
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
     </row>
-    <row r="57" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -1756,7 +1877,7 @@
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
     </row>
-    <row r="58" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -1770,7 +1891,7 @@
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
     </row>
-    <row r="59" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -1784,7 +1905,7 @@
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
     </row>
-    <row r="60" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -1798,7 +1919,7 @@
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
     </row>
-    <row r="61" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -1812,7 +1933,7 @@
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
     </row>
-    <row r="62" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -1826,7 +1947,7 @@
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
     </row>
-    <row r="63" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -1840,7 +1961,7 @@
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
     </row>
-    <row r="64" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -1854,7 +1975,7 @@
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
     </row>
-    <row r="65" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -1868,7 +1989,7 @@
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
     </row>
-    <row r="66" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -1882,7 +2003,7 @@
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
     </row>
-    <row r="67" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -1896,7 +2017,7 @@
       <c r="L67" s="1"/>
       <c r="M67" s="1"/>
     </row>
-    <row r="68" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -1910,7 +2031,7 @@
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
     </row>
-    <row r="69" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -1924,7 +2045,7 @@
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
     </row>
-    <row r="70" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -1938,7 +2059,7 @@
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
     </row>
-    <row r="71" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -1952,7 +2073,7 @@
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
     </row>
-    <row r="72" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -1966,7 +2087,7 @@
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
     </row>
-    <row r="73" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
@@ -1980,7 +2101,7 @@
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
     </row>
-    <row r="74" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -1994,7 +2115,7 @@
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
     </row>
-    <row r="75" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -2008,7 +2129,7 @@
       <c r="L75" s="1"/>
       <c r="M75" s="1"/>
     </row>
-    <row r="76" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -2022,7 +2143,7 @@
       <c r="L76" s="1"/>
       <c r="M76" s="1"/>
     </row>
-    <row r="77" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -2036,7 +2157,7 @@
       <c r="L77" s="1"/>
       <c r="M77" s="1"/>
     </row>
-    <row r="78" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -2050,7 +2171,7 @@
       <c r="L78" s="1"/>
       <c r="M78" s="1"/>
     </row>
-    <row r="79" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
@@ -2064,7 +2185,7 @@
       <c r="L79" s="1"/>
       <c r="M79" s="1"/>
     </row>
-    <row r="80" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
@@ -2078,7 +2199,7 @@
       <c r="L80" s="1"/>
       <c r="M80" s="1"/>
     </row>
-    <row r="81" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
@@ -2092,7 +2213,7 @@
       <c r="L81" s="1"/>
       <c r="M81" s="1"/>
     </row>
-    <row r="82" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
@@ -2106,7 +2227,7 @@
       <c r="L82" s="1"/>
       <c r="M82" s="1"/>
     </row>
-    <row r="83" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
@@ -2120,7 +2241,7 @@
       <c r="L83" s="1"/>
       <c r="M83" s="1"/>
     </row>
-    <row r="84" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
@@ -2134,7 +2255,7 @@
       <c r="L84" s="1"/>
       <c r="M84" s="1"/>
     </row>
-    <row r="85" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
@@ -2148,7 +2269,7 @@
       <c r="L85" s="1"/>
       <c r="M85" s="1"/>
     </row>
-    <row r="86" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
@@ -2162,7 +2283,7 @@
       <c r="L86" s="1"/>
       <c r="M86" s="1"/>
     </row>
-    <row r="87" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
@@ -2176,7 +2297,7 @@
       <c r="L87" s="1"/>
       <c r="M87" s="1"/>
     </row>
-    <row r="88" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
@@ -2190,7 +2311,7 @@
       <c r="L88" s="1"/>
       <c r="M88" s="1"/>
     </row>
-    <row r="89" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
@@ -2204,7 +2325,7 @@
       <c r="L89" s="1"/>
       <c r="M89" s="1"/>
     </row>
-    <row r="90" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
@@ -2218,7 +2339,7 @@
       <c r="L90" s="1"/>
       <c r="M90" s="1"/>
     </row>
-    <row r="91" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
@@ -2232,7 +2353,7 @@
       <c r="L91" s="1"/>
       <c r="M91" s="1"/>
     </row>
-    <row r="92" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
@@ -2246,7 +2367,7 @@
       <c r="L92" s="1"/>
       <c r="M92" s="1"/>
     </row>
-    <row r="93" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
@@ -2260,7 +2381,7 @@
       <c r="L93" s="1"/>
       <c r="M93" s="1"/>
     </row>
-    <row r="94" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
@@ -2274,7 +2395,7 @@
       <c r="L94" s="1"/>
       <c r="M94" s="1"/>
     </row>
-    <row r="95" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
@@ -2288,7 +2409,7 @@
       <c r="L95" s="1"/>
       <c r="M95" s="1"/>
     </row>
-    <row r="96" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
@@ -2302,7 +2423,7 @@
       <c r="L96" s="1"/>
       <c r="M96" s="1"/>
     </row>
-    <row r="97" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
@@ -2316,7 +2437,7 @@
       <c r="L97" s="1"/>
       <c r="M97" s="1"/>
     </row>
-    <row r="98" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
@@ -2330,7 +2451,7 @@
       <c r="L98" s="1"/>
       <c r="M98" s="1"/>
     </row>
-    <row r="99" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
@@ -2344,7 +2465,7 @@
       <c r="L99" s="1"/>
       <c r="M99" s="1"/>
     </row>
-    <row r="100" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
@@ -2358,7 +2479,7 @@
       <c r="L100" s="1"/>
       <c r="M100" s="1"/>
     </row>
-    <row r="101" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
@@ -2372,7 +2493,7 @@
       <c r="L101" s="1"/>
       <c r="M101" s="1"/>
     </row>
-    <row r="102" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
@@ -2386,7 +2507,7 @@
       <c r="L102" s="1"/>
       <c r="M102" s="1"/>
     </row>
-    <row r="103" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
@@ -2400,7 +2521,7 @@
       <c r="L103" s="1"/>
       <c r="M103" s="1"/>
     </row>
-    <row r="104" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
@@ -2414,7 +2535,7 @@
       <c r="L104" s="1"/>
       <c r="M104" s="1"/>
     </row>
-    <row r="105" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
@@ -2428,7 +2549,7 @@
       <c r="L105" s="1"/>
       <c r="M105" s="1"/>
     </row>
-    <row r="106" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
@@ -2442,7 +2563,7 @@
       <c r="L106" s="1"/>
       <c r="M106" s="1"/>
     </row>
-    <row r="107" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
@@ -2456,7 +2577,7 @@
       <c r="L107" s="1"/>
       <c r="M107" s="1"/>
     </row>
-    <row r="108" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
@@ -2470,7 +2591,7 @@
       <c r="L108" s="1"/>
       <c r="M108" s="1"/>
     </row>
-    <row r="109" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
@@ -2484,7 +2605,7 @@
       <c r="L109" s="1"/>
       <c r="M109" s="1"/>
     </row>
-    <row r="110" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
@@ -2498,7 +2619,7 @@
       <c r="L110" s="1"/>
       <c r="M110" s="1"/>
     </row>
-    <row r="111" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
@@ -2512,7 +2633,7 @@
       <c r="L111" s="1"/>
       <c r="M111" s="1"/>
     </row>
-    <row r="112" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
@@ -2526,7 +2647,7 @@
       <c r="L112" s="1"/>
       <c r="M112" s="1"/>
     </row>
-    <row r="113" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
@@ -2540,7 +2661,7 @@
       <c r="L113" s="1"/>
       <c r="M113" s="1"/>
     </row>
-    <row r="114" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
@@ -2554,7 +2675,7 @@
       <c r="L114" s="1"/>
       <c r="M114" s="1"/>
     </row>
-    <row r="115" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
@@ -2568,7 +2689,7 @@
       <c r="L115" s="1"/>
       <c r="M115" s="1"/>
     </row>
-    <row r="116" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
@@ -2582,7 +2703,7 @@
       <c r="L116" s="1"/>
       <c r="M116" s="1"/>
     </row>
-    <row r="117" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
@@ -2596,7 +2717,7 @@
       <c r="L117" s="1"/>
       <c r="M117" s="1"/>
     </row>
-    <row r="118" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
@@ -2610,7 +2731,7 @@
       <c r="L118" s="1"/>
       <c r="M118" s="1"/>
     </row>
-    <row r="119" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
@@ -2624,7 +2745,7 @@
       <c r="L119" s="1"/>
       <c r="M119" s="1"/>
     </row>
-    <row r="120" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
@@ -2638,7 +2759,7 @@
       <c r="L120" s="1"/>
       <c r="M120" s="1"/>
     </row>
-    <row r="121" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
@@ -2652,7 +2773,7 @@
       <c r="L121" s="1"/>
       <c r="M121" s="1"/>
     </row>
-    <row r="122" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
@@ -2666,7 +2787,7 @@
       <c r="L122" s="1"/>
       <c r="M122" s="1"/>
     </row>
-    <row r="123" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
@@ -2680,7 +2801,7 @@
       <c r="L123" s="1"/>
       <c r="M123" s="1"/>
     </row>
-    <row r="124" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
@@ -2694,7 +2815,7 @@
       <c r="L124" s="1"/>
       <c r="M124" s="1"/>
     </row>
-    <row r="125" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
@@ -2708,7 +2829,7 @@
       <c r="L125" s="1"/>
       <c r="M125" s="1"/>
     </row>
-    <row r="126" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
@@ -2722,7 +2843,7 @@
       <c r="L126" s="1"/>
       <c r="M126" s="1"/>
     </row>
-    <row r="127" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
@@ -2736,7 +2857,7 @@
       <c r="L127" s="1"/>
       <c r="M127" s="1"/>
     </row>
-    <row r="128" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
@@ -2750,7 +2871,7 @@
       <c r="L128" s="1"/>
       <c r="M128" s="1"/>
     </row>
-    <row r="129" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
@@ -2764,7 +2885,7 @@
       <c r="L129" s="1"/>
       <c r="M129" s="1"/>
     </row>
-    <row r="130" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
@@ -2778,7 +2899,7 @@
       <c r="L130" s="1"/>
       <c r="M130" s="1"/>
     </row>
-    <row r="131" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
@@ -2792,7 +2913,7 @@
       <c r="L131" s="1"/>
       <c r="M131" s="1"/>
     </row>
-    <row r="132" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
@@ -2806,7 +2927,7 @@
       <c r="L132" s="1"/>
       <c r="M132" s="1"/>
     </row>
-    <row r="133" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
@@ -2820,7 +2941,7 @@
       <c r="L133" s="1"/>
       <c r="M133" s="1"/>
     </row>
-    <row r="134" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
@@ -2834,7 +2955,7 @@
       <c r="L134" s="1"/>
       <c r="M134" s="1"/>
     </row>
-    <row r="135" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
@@ -2848,7 +2969,7 @@
       <c r="L135" s="1"/>
       <c r="M135" s="1"/>
     </row>
-    <row r="136" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
       <c r="D136" s="1"/>
@@ -2862,7 +2983,7 @@
       <c r="L136" s="1"/>
       <c r="M136" s="1"/>
     </row>
-    <row r="137" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
@@ -2876,7 +2997,7 @@
       <c r="L137" s="1"/>
       <c r="M137" s="1"/>
     </row>
-    <row r="138" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
@@ -2890,7 +3011,7 @@
       <c r="L138" s="1"/>
       <c r="M138" s="1"/>
     </row>
-    <row r="139" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
@@ -2904,7 +3025,7 @@
       <c r="L139" s="1"/>
       <c r="M139" s="1"/>
     </row>
-    <row r="140" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
@@ -2918,7 +3039,7 @@
       <c r="L140" s="1"/>
       <c r="M140" s="1"/>
     </row>
-    <row r="141" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
       <c r="D141" s="1"/>
@@ -2932,7 +3053,7 @@
       <c r="L141" s="1"/>
       <c r="M141" s="1"/>
     </row>
-    <row r="142" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
@@ -2946,7 +3067,7 @@
       <c r="L142" s="1"/>
       <c r="M142" s="1"/>
     </row>
-    <row r="143" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
@@ -2960,7 +3081,7 @@
       <c r="L143" s="1"/>
       <c r="M143" s="1"/>
     </row>
-    <row r="144" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
       <c r="D144" s="1"/>
@@ -2974,7 +3095,7 @@
       <c r="L144" s="1"/>
       <c r="M144" s="1"/>
     </row>
-    <row r="145" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
       <c r="D145" s="1"/>
@@ -2988,7 +3109,7 @@
       <c r="L145" s="1"/>
       <c r="M145" s="1"/>
     </row>
-    <row r="146" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
       <c r="D146" s="1"/>
@@ -3002,7 +3123,7 @@
       <c r="L146" s="1"/>
       <c r="M146" s="1"/>
     </row>
-    <row r="147" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
       <c r="D147" s="1"/>
@@ -3016,7 +3137,7 @@
       <c r="L147" s="1"/>
       <c r="M147" s="1"/>
     </row>
-    <row r="148" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
       <c r="D148" s="1"/>
@@ -3030,7 +3151,7 @@
       <c r="L148" s="1"/>
       <c r="M148" s="1"/>
     </row>
-    <row r="149" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
       <c r="D149" s="1"/>
@@ -3044,7 +3165,7 @@
       <c r="L149" s="1"/>
       <c r="M149" s="1"/>
     </row>
-    <row r="150" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
       <c r="D150" s="1"/>
@@ -3058,7 +3179,7 @@
       <c r="L150" s="1"/>
       <c r="M150" s="1"/>
     </row>
-    <row r="151" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
       <c r="D151" s="1"/>
@@ -3072,7 +3193,7 @@
       <c r="L151" s="1"/>
       <c r="M151" s="1"/>
     </row>
-    <row r="152" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
       <c r="D152" s="1"/>
@@ -3086,7 +3207,7 @@
       <c r="L152" s="1"/>
       <c r="M152" s="1"/>
     </row>
-    <row r="153" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
       <c r="D153" s="1"/>
@@ -3100,7 +3221,7 @@
       <c r="L153" s="1"/>
       <c r="M153" s="1"/>
     </row>
-    <row r="154" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
       <c r="D154" s="1"/>
@@ -3114,7 +3235,7 @@
       <c r="L154" s="1"/>
       <c r="M154" s="1"/>
     </row>
-    <row r="155" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
       <c r="D155" s="1"/>
@@ -3128,7 +3249,7 @@
       <c r="L155" s="1"/>
       <c r="M155" s="1"/>
     </row>
-    <row r="156" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
       <c r="D156" s="1"/>
@@ -3142,7 +3263,7 @@
       <c r="L156" s="1"/>
       <c r="M156" s="1"/>
     </row>
-    <row r="157" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
       <c r="D157" s="1"/>
@@ -3156,7 +3277,7 @@
       <c r="L157" s="1"/>
       <c r="M157" s="1"/>
     </row>
-    <row r="158" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
       <c r="D158" s="1"/>
@@ -3170,7 +3291,7 @@
       <c r="L158" s="1"/>
       <c r="M158" s="1"/>
     </row>
-    <row r="159" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
       <c r="D159" s="1"/>
@@ -3184,7 +3305,7 @@
       <c r="L159" s="1"/>
       <c r="M159" s="1"/>
     </row>
-    <row r="160" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
       <c r="D160" s="1"/>
@@ -3198,7 +3319,7 @@
       <c r="L160" s="1"/>
       <c r="M160" s="1"/>
     </row>
-    <row r="161" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
       <c r="D161" s="1"/>
@@ -3212,7 +3333,7 @@
       <c r="L161" s="1"/>
       <c r="M161" s="1"/>
     </row>
-    <row r="162" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
       <c r="D162" s="1"/>
@@ -3226,7 +3347,7 @@
       <c r="L162" s="1"/>
       <c r="M162" s="1"/>
     </row>
-    <row r="163" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
       <c r="D163" s="1"/>
@@ -3240,7 +3361,7 @@
       <c r="L163" s="1"/>
       <c r="M163" s="1"/>
     </row>
-    <row r="164" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
       <c r="D164" s="1"/>
@@ -3254,7 +3375,7 @@
       <c r="L164" s="1"/>
       <c r="M164" s="1"/>
     </row>
-    <row r="165" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
       <c r="D165" s="1"/>
@@ -3268,7 +3389,7 @@
       <c r="L165" s="1"/>
       <c r="M165" s="1"/>
     </row>
-    <row r="166" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
       <c r="D166" s="1"/>
@@ -3282,7 +3403,7 @@
       <c r="L166" s="1"/>
       <c r="M166" s="1"/>
     </row>
-    <row r="167" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
       <c r="D167" s="1"/>
@@ -3296,7 +3417,7 @@
       <c r="L167" s="1"/>
       <c r="M167" s="1"/>
     </row>
-    <row r="168" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
       <c r="D168" s="1"/>
@@ -3310,7 +3431,7 @@
       <c r="L168" s="1"/>
       <c r="M168" s="1"/>
     </row>
-    <row r="169" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
       <c r="D169" s="1"/>
@@ -3324,7 +3445,7 @@
       <c r="L169" s="1"/>
       <c r="M169" s="1"/>
     </row>
-    <row r="170" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
       <c r="D170" s="1"/>
@@ -3338,7 +3459,7 @@
       <c r="L170" s="1"/>
       <c r="M170" s="1"/>
     </row>
-    <row r="171" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
       <c r="D171" s="1"/>
@@ -3352,7 +3473,7 @@
       <c r="L171" s="1"/>
       <c r="M171" s="1"/>
     </row>
-    <row r="172" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
       <c r="D172" s="1"/>
@@ -3366,7 +3487,7 @@
       <c r="L172" s="1"/>
       <c r="M172" s="1"/>
     </row>
-    <row r="173" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
       <c r="D173" s="1"/>
@@ -3380,7 +3501,7 @@
       <c r="L173" s="1"/>
       <c r="M173" s="1"/>
     </row>
-    <row r="174" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
       <c r="D174" s="1"/>
@@ -3394,7 +3515,7 @@
       <c r="L174" s="1"/>
       <c r="M174" s="1"/>
     </row>
-    <row r="175" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
       <c r="D175" s="1"/>
@@ -3408,7 +3529,7 @@
       <c r="L175" s="1"/>
       <c r="M175" s="1"/>
     </row>
-    <row r="176" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
       <c r="D176" s="1"/>
@@ -3422,7 +3543,7 @@
       <c r="L176" s="1"/>
       <c r="M176" s="1"/>
     </row>
-    <row r="177" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
       <c r="D177" s="1"/>
@@ -3436,7 +3557,7 @@
       <c r="L177" s="1"/>
       <c r="M177" s="1"/>
     </row>
-    <row r="178" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
       <c r="D178" s="1"/>
@@ -3450,7 +3571,7 @@
       <c r="L178" s="1"/>
       <c r="M178" s="1"/>
     </row>
-    <row r="179" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
       <c r="D179" s="1"/>
@@ -3464,7 +3585,7 @@
       <c r="L179" s="1"/>
       <c r="M179" s="1"/>
     </row>
-    <row r="180" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
       <c r="D180" s="1"/>
@@ -3478,7 +3599,7 @@
       <c r="L180" s="1"/>
       <c r="M180" s="1"/>
     </row>
-    <row r="181" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
       <c r="D181" s="1"/>
@@ -3492,7 +3613,7 @@
       <c r="L181" s="1"/>
       <c r="M181" s="1"/>
     </row>
-    <row r="182" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
       <c r="D182" s="1"/>
@@ -3506,7 +3627,7 @@
       <c r="L182" s="1"/>
       <c r="M182" s="1"/>
     </row>
-    <row r="183" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
       <c r="D183" s="1"/>
@@ -3520,7 +3641,7 @@
       <c r="L183" s="1"/>
       <c r="M183" s="1"/>
     </row>
-    <row r="184" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
       <c r="D184" s="1"/>
@@ -3534,7 +3655,7 @@
       <c r="L184" s="1"/>
       <c r="M184" s="1"/>
     </row>
-    <row r="185" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
       <c r="D185" s="1"/>
@@ -3548,7 +3669,7 @@
       <c r="L185" s="1"/>
       <c r="M185" s="1"/>
     </row>
-    <row r="186" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
       <c r="D186" s="1"/>
@@ -3562,7 +3683,7 @@
       <c r="L186" s="1"/>
       <c r="M186" s="1"/>
     </row>
-    <row r="187" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
       <c r="D187" s="1"/>
@@ -3576,7 +3697,7 @@
       <c r="L187" s="1"/>
       <c r="M187" s="1"/>
     </row>
-    <row r="188" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
       <c r="D188" s="1"/>
@@ -3590,7 +3711,7 @@
       <c r="L188" s="1"/>
       <c r="M188" s="1"/>
     </row>
-    <row r="189" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
       <c r="D189" s="1"/>
@@ -3604,7 +3725,7 @@
       <c r="L189" s="1"/>
       <c r="M189" s="1"/>
     </row>
-    <row r="190" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
       <c r="D190" s="1"/>
@@ -3618,7 +3739,7 @@
       <c r="L190" s="1"/>
       <c r="M190" s="1"/>
     </row>
-    <row r="191" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
       <c r="D191" s="1"/>
@@ -3632,7 +3753,7 @@
       <c r="L191" s="1"/>
       <c r="M191" s="1"/>
     </row>
-    <row r="192" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
       <c r="D192" s="1"/>
@@ -3646,7 +3767,7 @@
       <c r="L192" s="1"/>
       <c r="M192" s="1"/>
     </row>
-    <row r="193" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
       <c r="D193" s="1"/>
@@ -3660,7 +3781,7 @@
       <c r="L193" s="1"/>
       <c r="M193" s="1"/>
     </row>
-    <row r="194" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
       <c r="D194" s="1"/>
@@ -3674,7 +3795,7 @@
       <c r="L194" s="1"/>
       <c r="M194" s="1"/>
     </row>
-    <row r="195" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
       <c r="D195" s="1"/>
@@ -3688,7 +3809,7 @@
       <c r="L195" s="1"/>
       <c r="M195" s="1"/>
     </row>
-    <row r="196" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
       <c r="D196" s="1"/>
@@ -3702,7 +3823,7 @@
       <c r="L196" s="1"/>
       <c r="M196" s="1"/>
     </row>
-    <row r="197" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
       <c r="D197" s="1"/>
@@ -3716,7 +3837,7 @@
       <c r="L197" s="1"/>
       <c r="M197" s="1"/>
     </row>
-    <row r="198" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
       <c r="D198" s="1"/>
@@ -3730,7 +3851,7 @@
       <c r="L198" s="1"/>
       <c r="M198" s="1"/>
     </row>
-    <row r="199" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
       <c r="D199" s="1"/>
@@ -3744,7 +3865,7 @@
       <c r="L199" s="1"/>
       <c r="M199" s="1"/>
     </row>
-    <row r="200" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
       <c r="D200" s="1"/>
@@ -3758,7 +3879,7 @@
       <c r="L200" s="1"/>
       <c r="M200" s="1"/>
     </row>
-    <row r="201" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
       <c r="D201" s="1"/>
@@ -3772,7 +3893,7 @@
       <c r="L201" s="1"/>
       <c r="M201" s="1"/>
     </row>
-    <row r="202" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
       <c r="D202" s="1"/>
@@ -3786,7 +3907,7 @@
       <c r="L202" s="1"/>
       <c r="M202" s="1"/>
     </row>
-    <row r="203" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
       <c r="D203" s="1"/>
@@ -3800,7 +3921,7 @@
       <c r="L203" s="1"/>
       <c r="M203" s="1"/>
     </row>
-    <row r="204" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
       <c r="D204" s="1"/>
@@ -3814,7 +3935,7 @@
       <c r="L204" s="1"/>
       <c r="M204" s="1"/>
     </row>
-    <row r="205" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
       <c r="D205" s="1"/>
@@ -3828,7 +3949,7 @@
       <c r="L205" s="1"/>
       <c r="M205" s="1"/>
     </row>
-    <row r="206" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
       <c r="D206" s="1"/>
@@ -3842,7 +3963,7 @@
       <c r="L206" s="1"/>
       <c r="M206" s="1"/>
     </row>
-    <row r="207" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
       <c r="D207" s="1"/>
@@ -3856,7 +3977,7 @@
       <c r="L207" s="1"/>
       <c r="M207" s="1"/>
     </row>
-    <row r="208" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
       <c r="D208" s="1"/>
@@ -3870,7 +3991,7 @@
       <c r="L208" s="1"/>
       <c r="M208" s="1"/>
     </row>
-    <row r="209" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
       <c r="D209" s="1"/>
@@ -3884,7 +4005,7 @@
       <c r="L209" s="1"/>
       <c r="M209" s="1"/>
     </row>
-    <row r="210" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
       <c r="D210" s="1"/>
@@ -3898,7 +4019,7 @@
       <c r="L210" s="1"/>
       <c r="M210" s="1"/>
     </row>
-    <row r="211" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
       <c r="D211" s="1"/>
@@ -3912,7 +4033,7 @@
       <c r="L211" s="1"/>
       <c r="M211" s="1"/>
     </row>
-    <row r="212" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
       <c r="D212" s="1"/>
@@ -3926,7 +4047,7 @@
       <c r="L212" s="1"/>
       <c r="M212" s="1"/>
     </row>
-    <row r="213" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
       <c r="D213" s="1"/>
@@ -3940,7 +4061,7 @@
       <c r="L213" s="1"/>
       <c r="M213" s="1"/>
     </row>
-    <row r="214" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
       <c r="D214" s="1"/>
@@ -3954,7 +4075,7 @@
       <c r="L214" s="1"/>
       <c r="M214" s="1"/>
     </row>
-    <row r="215" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
       <c r="D215" s="1"/>
@@ -3968,7 +4089,7 @@
       <c r="L215" s="1"/>
       <c r="M215" s="1"/>
     </row>
-    <row r="216" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
       <c r="D216" s="1"/>
@@ -3982,7 +4103,7 @@
       <c r="L216" s="1"/>
       <c r="M216" s="1"/>
     </row>
-    <row r="217" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
       <c r="D217" s="1"/>
@@ -3996,7 +4117,7 @@
       <c r="L217" s="1"/>
       <c r="M217" s="1"/>
     </row>
-    <row r="218" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
       <c r="D218" s="1"/>
@@ -4010,37 +4131,79 @@
       <c r="L218" s="1"/>
       <c r="M218" s="1"/>
     </row>
+    <row r="219" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B219" s="1"/>
+      <c r="C219" s="1"/>
+      <c r="D219" s="1"/>
+      <c r="E219" s="1"/>
+      <c r="F219" s="1"/>
+      <c r="G219" s="1"/>
+      <c r="H219" s="1"/>
+      <c r="I219" s="1"/>
+      <c r="J219" s="1"/>
+      <c r="K219" s="1"/>
+      <c r="L219" s="1"/>
+      <c r="M219" s="1"/>
+    </row>
+    <row r="220" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B220" s="1"/>
+      <c r="C220" s="1"/>
+      <c r="D220" s="1"/>
+      <c r="E220" s="1"/>
+      <c r="F220" s="1"/>
+      <c r="G220" s="1"/>
+      <c r="H220" s="1"/>
+      <c r="I220" s="1"/>
+      <c r="J220" s="1"/>
+      <c r="K220" s="1"/>
+      <c r="L220" s="1"/>
+      <c r="M220" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B30:C31"/>
-    <mergeCell ref="A26:L26"/>
-    <mergeCell ref="A21:L21"/>
-    <mergeCell ref="A22:L22"/>
-    <mergeCell ref="A23:L23"/>
-    <mergeCell ref="A24:L24"/>
-    <mergeCell ref="A25:L25"/>
-    <mergeCell ref="A16:L16"/>
-    <mergeCell ref="A17:L17"/>
-    <mergeCell ref="A18:L18"/>
-    <mergeCell ref="A19:L19"/>
-    <mergeCell ref="A20:L20"/>
+  <mergeCells count="43">
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="M3:N3"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A1:L1"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="A28:L28"/>
+    <mergeCell ref="A23:L23"/>
+    <mergeCell ref="A24:L24"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="A26:L26"/>
+    <mergeCell ref="A27:L27"/>
+    <mergeCell ref="A18:L18"/>
+    <mergeCell ref="A19:L19"/>
+    <mergeCell ref="A20:L20"/>
+    <mergeCell ref="A21:L21"/>
+    <mergeCell ref="A22:L22"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="M8:N9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>